<commit_message>
most of Xbee sender code done (except for command check and checking acknowledgements)
</commit_message>
<xml_diff>
--- a/finalproject_811 (bill of materials CSV).xlsx
+++ b/finalproject_811 (bill of materials CSV).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="82">
   <si>
     <t>Component</t>
   </si>
@@ -245,9 +245,6 @@
   </si>
   <si>
     <t>2.7 ma</t>
-  </si>
-  <si>
-    <t>C2 C10 C12</t>
   </si>
   <si>
     <t>TLV5618</t>
@@ -1071,8 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,19 +1571,13 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H33" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I33">
         <v>1</v>
@@ -1594,13 +1585,13 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="H34" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -1608,61 +1599,64 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H35" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I35">
         <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1.63</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="H36" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="I36">
         <v>1</v>
       </c>
       <c r="K36">
-        <v>1.63</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="H37" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I37">
         <v>1</v>
       </c>
-      <c r="K37">
-        <v>0.23</v>
+      <c r="J37" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="H38" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="I38">
         <v>1</v>
@@ -1670,13 +1664,13 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="H39" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="I39">
         <v>1</v>
@@ -1684,131 +1678,36 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="H40" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="I40">
         <v>1</v>
-      </c>
-      <c r="J40" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" t="s">
-        <v>81</v>
-      </c>
-      <c r="H41" t="s">
-        <v>82</v>
+        <v>55</v>
+      </c>
+      <c r="D41" t="s">
+        <v>56</v>
       </c>
       <c r="I41">
         <v>1</v>
       </c>
+      <c r="K41">
+        <v>20</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>16</v>
-      </c>
-      <c r="H42" t="s">
-        <v>77</v>
-      </c>
-      <c r="I42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" t="s">
-        <v>19</v>
-      </c>
-      <c r="H43" t="s">
-        <v>44</v>
-      </c>
-      <c r="I43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" t="s">
-        <v>45</v>
-      </c>
-      <c r="H44" t="s">
-        <v>46</v>
-      </c>
-      <c r="I44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" t="s">
-        <v>47</v>
-      </c>
-      <c r="H45" t="s">
-        <v>48</v>
-      </c>
-      <c r="I45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B46" t="s">
-        <v>13</v>
-      </c>
-      <c r="H46" t="s">
-        <v>79</v>
-      </c>
-      <c r="I46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>52</v>
-      </c>
-      <c r="B47" t="s">
-        <v>53</v>
-      </c>
-      <c r="H47" t="s">
-        <v>54</v>
-      </c>
-      <c r="I47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>55</v>
-      </c>
-      <c r="D48" t="s">
-        <v>56</v>
-      </c>
-      <c r="I48">
-        <v>1</v>
-      </c>
-      <c r="K48">
-        <v>20</v>
+      <c r="K42">
+        <f>SUM(K2:K41)</f>
+        <v>23.86</v>
       </c>
     </row>
     <row r="49" spans="9:11" x14ac:dyDescent="0.25">
@@ -1821,12 +1720,12 @@
     </row>
     <row r="50" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I50">
-        <f>SUM(I2:I48)</f>
-        <v>78</v>
+        <f>SUM(I2:I45)</f>
+        <v>69</v>
       </c>
       <c r="K50">
-        <f>SUM(K1:K48)</f>
-        <v>23.86</v>
+        <f>SUM(K1:K45)</f>
+        <v>47.72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>